<commit_message>
Correction of files - old files had been uploaded
Correct files for the WEB detailed analysis differences in Phase 2 uploaded.
</commit_message>
<xml_diff>
--- a/Phase 2/Freqsal/WEB/Detailed analysis/web_freq5sal49_200310.xlsx
+++ b/Phase 2/Freqsal/WEB/Detailed analysis/web_freq5sal49_200310.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Dropbox\Light\Doctorate\Data_and_scripts\March_crazed_panic\Method-eval_update\Freq_sal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Documents\GitHub\Appendices\Phase 2\Freqsal\WEB\Detailed analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCF8CB9-9DF6-455B-B8F9-73C44CC41434}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC85186-16CD-446C-9E4F-F971C7535D29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3481,7 +3483,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="83" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -3493,7 +3495,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308523" cy="6090227"/>
+    <xdr:ext cx="9306958" cy="6082229"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4683,7 +4685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
@@ -6032,7 +6034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -8001,7 +8003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>